<commit_message>
finished analysis of couter flow heat exchangers
</commit_message>
<xml_diff>
--- a/Lab10_HeatExchanger/HeatExchangerTables-Blank.xlsx
+++ b/Lab10_HeatExchanger/HeatExchangerTables-Blank.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/professor/Teaching/ME4650/Labs/HeatExchanger/Handout/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jfrancis/Documents/GitHub/thermalFluidEnergySystems/Lab10_HeatExchanger/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EE3587-CA38-1F49-8B40-5E4CCEB7138C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D507C0-C892-A246-A5BB-F3E99F0309D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1720" windowWidth="19120" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1720" windowWidth="25740" windowHeight="13860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1a" sheetId="2" r:id="rId1"/>
@@ -207,7 +207,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -253,13 +253,6 @@
       <color theme="1"/>
       <name val="Symbol"/>
       <charset val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1" tint="0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -756,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -779,118 +772,100 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -902,15 +877,6 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -947,37 +913,37 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1049,9 +1015,9 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>545867</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>48455</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="246944" cy="177800"/>
@@ -1088,9 +1054,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>520465</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>55841</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="247650" cy="173355"/>
@@ -1127,15 +1093,15 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>339652</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>49539</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>511102</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>241710</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1171,15 +1137,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>332269</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>59975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>515149</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>233096</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1215,15 +1181,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>162442</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>45207</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>417712</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>271668</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1259,15 +1225,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>236279</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>45206</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>605849</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>252617</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1303,15 +1269,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>199360</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>37822</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>557500</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>245233</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1352,9 +1318,9 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>375658</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>48455</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="246944" cy="177800"/>
@@ -1391,9 +1357,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>350256</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>55841</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="247650" cy="173355"/>
@@ -1731,144 +1697,209 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="B1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24" customHeight="1">
-      <c r="A1" s="64" t="s">
+    <row r="1" spans="2:12" ht="17" thickBot="1"/>
+    <row r="2" spans="2:12" ht="24" customHeight="1">
+      <c r="B2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="C2" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="66" t="s">
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="68"/>
-      <c r="H1" s="69" t="s">
+      <c r="H2" s="59"/>
+      <c r="I2" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="J2" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="67"/>
-      <c r="K1" s="68"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="59"/>
     </row>
-    <row r="2" spans="1:11" ht="24" customHeight="1" thickBot="1">
-      <c r="A2" s="65"/>
-      <c r="B2" s="71"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="18" t="s">
+    <row r="3" spans="2:12" ht="24" customHeight="1" thickBot="1">
+      <c r="B3" s="56"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="19" t="s">
+    <row r="4" spans="2:12">
+      <c r="B4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="20" t="s">
+      <c r="C4" s="22">
+        <v>0.17660000000000001</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="21" t="s">
+      <c r="E4" s="25">
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="37"/>
+      <c r="G4" s="28">
+        <v>5.1660000000000004</v>
+      </c>
+      <c r="H4" s="29">
+        <v>6.78</v>
+      </c>
+      <c r="I4" s="22">
+        <v>5290</v>
+      </c>
+      <c r="J4" s="28">
+        <v>-6.54</v>
+      </c>
+      <c r="K4" s="30">
+        <v>6.58</v>
+      </c>
+      <c r="L4" s="31">
+        <v>0.95</v>
+      </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="22" t="s">
+    <row r="5" spans="2:12">
+      <c r="B5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="23" t="s">
+      <c r="C5" s="23">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="24" t="s">
+      <c r="E5" s="26">
+        <v>0.128</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="41"/>
+      <c r="G5" s="32">
+        <v>7</v>
+      </c>
+      <c r="H5" s="33">
+        <v>6.78</v>
+      </c>
+      <c r="I5" s="23">
+        <v>4670</v>
+      </c>
+      <c r="J5" s="32">
+        <v>-6.37</v>
+      </c>
+      <c r="K5" s="34">
+        <v>5.72</v>
+      </c>
+      <c r="L5" s="35">
+        <v>10.64</v>
+      </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="22" t="s">
+    <row r="6" spans="2:12">
+      <c r="B6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="23" t="s">
+      <c r="C6" s="23">
+        <v>0.1487</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="24" t="s">
+      <c r="E6" s="26">
+        <v>0.22140000000000001</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="38"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="41"/>
+      <c r="G6" s="32">
+        <v>4</v>
+      </c>
+      <c r="H6" s="33">
+        <v>7.17</v>
+      </c>
+      <c r="I6" s="23">
+        <v>4580</v>
+      </c>
+      <c r="J6" s="32">
+        <v>-5.82</v>
+      </c>
+      <c r="K6" s="34">
+        <v>5.67</v>
+      </c>
+      <c r="L6" s="35">
+        <v>2.57</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" ht="17" thickBot="1">
-      <c r="A6" s="25" t="s">
+    <row r="7" spans="2:12" ht="17" thickBot="1">
+      <c r="B7" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="26" t="s">
+      <c r="C7" s="24">
+        <v>0.15809999999999999</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="27" t="s">
+      <c r="E7" s="27">
+        <v>0.1278</v>
+      </c>
+      <c r="F7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="45"/>
+      <c r="G7" s="36">
+        <v>6.89</v>
+      </c>
+      <c r="H7" s="37">
+        <v>7</v>
+      </c>
+      <c r="I7" s="24">
+        <v>4530</v>
+      </c>
+      <c r="J7" s="36">
+        <v>-6.04</v>
+      </c>
+      <c r="K7" s="38">
+        <v>5.64</v>
+      </c>
+      <c r="L7" s="39">
+        <v>6.9</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="83" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1881,143 +1912,200 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" style="1" customWidth="1"/>
-    <col min="6" max="9" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="6.1640625" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" style="1" customWidth="1"/>
+    <col min="7" max="10" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25" customHeight="1">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="2:11" ht="17" thickBot="1"/>
+    <row r="2" spans="2:11" ht="25" customHeight="1">
+      <c r="B2" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="C2" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="80" t="s">
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="82" t="s">
+      <c r="H2" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="84" t="s">
+      <c r="I2" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="85"/>
-      <c r="J1" s="86"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="77"/>
     </row>
-    <row r="2" spans="1:10" ht="25" customHeight="1" thickBot="1">
-      <c r="A2" s="76"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="5" t="s">
+    <row r="3" spans="2:11" ht="25" customHeight="1" thickBot="1">
+      <c r="B3" s="67"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="2:11">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="8" t="s">
+      <c r="C4" s="22">
+        <v>0.17660000000000001</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="9" t="s">
+      <c r="E4" s="25">
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="52"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="55"/>
+      <c r="G4" s="43">
+        <v>0.76949999999999996</v>
+      </c>
+      <c r="H4" s="40">
+        <v>0.27589999999999998</v>
+      </c>
+      <c r="I4" s="44">
+        <v>0.2283</v>
+      </c>
+      <c r="J4" s="45">
+        <v>0.22170000000000001</v>
+      </c>
+      <c r="K4" s="46">
+        <v>2.9815999999999998</v>
+      </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="3" t="s">
+    <row r="5" spans="2:11">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="10" t="s">
+      <c r="C5" s="23">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="11" t="s">
+      <c r="E5" s="26">
+        <v>0.128</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="56"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="59"/>
+      <c r="G5" s="47">
+        <v>0.87050000000000005</v>
+      </c>
+      <c r="H5" s="41">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="I5" s="48">
+        <v>0.1961</v>
+      </c>
+      <c r="J5" s="49">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="K5" s="50">
+        <v>0.97230000000000005</v>
+      </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="2:11">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="10" t="s">
+      <c r="C6" s="23">
+        <v>0.1487</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="50"/>
-      <c r="E5" s="11" t="s">
+      <c r="E6" s="26">
+        <v>0.22140000000000001</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="56"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="59"/>
+      <c r="G6" s="47">
+        <v>0.57269999999999999</v>
+      </c>
+      <c r="H6" s="41">
+        <v>0.2387</v>
+      </c>
+      <c r="I6" s="48">
+        <v>0.2001</v>
+      </c>
+      <c r="J6" s="49">
+        <v>0.20080000000000001</v>
+      </c>
+      <c r="K6" s="50">
+        <v>0.38479999999999998</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" ht="17" thickBot="1">
-      <c r="A6" s="4" t="s">
+    <row r="7" spans="2:11" ht="17" thickBot="1">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="12" t="s">
+      <c r="C7" s="24">
+        <v>0.15809999999999999</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="51"/>
-      <c r="E6" s="13" t="s">
+      <c r="E7" s="27">
+        <v>0.1278</v>
+      </c>
+      <c r="F7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="60"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="63"/>
+      <c r="G7" s="51">
+        <v>0.94830000000000003</v>
+      </c>
+      <c r="H7" s="42">
+        <v>0.23569999999999999</v>
+      </c>
+      <c r="I7" s="52">
+        <v>0.1905</v>
+      </c>
+      <c r="J7" s="53">
+        <v>0.19170000000000001</v>
+      </c>
+      <c r="K7" s="54">
+        <v>0.64490000000000003</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="91" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>